<commit_message>
Process finished, tested, and checked in UiPath academy
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\UiPath\UiPathCertif_CalculateClientSecurityHash\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jureyes\Documents\UiPath\UiPathCertif_CalculateClientSecurityHash\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B9356B2-7FDF-42B7-B267-D3ED02B9EBED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="-28920" yWindow="-9270" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="79">
   <si>
     <t>Name</t>
   </si>
@@ -242,12 +243,30 @@
   </si>
   <si>
     <t>Get security hash from string</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>reyes.juanluis.perez@gmail.com</t>
+  </si>
+  <si>
+    <t>ACME Username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>DmnSlyr_14</t>
+  </si>
+  <si>
+    <t>ACME Password</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -293,17 +312,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -617,11 +635,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -683,7 +701,7 @@
       <c r="A5" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" t="s">
         <v>40</v>
       </c>
       <c r="C5" t="s">
@@ -705,7 +723,7 @@
       <c r="A7" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" t="s">
         <v>46</v>
       </c>
       <c r="C7" t="s">
@@ -727,7 +745,7 @@
       <c r="A9" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" t="s">
         <v>52</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -738,7 +756,7 @@
       <c r="A10" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" t="s">
         <v>67</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -782,15 +800,35 @@
       <c r="A14" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" t="s">
         <v>70</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
     <row r="17" spans="2:2" ht="14.25" customHeight="1"/>
     <row r="18" spans="2:2" ht="14.25" customHeight="1"/>
     <row r="19" spans="2:2" ht="14.25" customHeight="1"/>
@@ -1782,7 +1820,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2945,7 +2983,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -4000,7 +4038,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>